<commit_message>
Added density values to materials data
</commit_message>
<xml_diff>
--- a/data/material-properties-database.xlsx
+++ b/data/material-properties-database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repos\Steel Shapes Excel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0982CDD5-1815-44B6-AB30-5099420944DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C31297D-1998-48E3-B5E0-21935D18854C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="21000" xr2:uid="{A7C2A3F0-3DCD-45CF-9C3E-C688DFDCAF82}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Grade</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>HPS 100W</t>
+  </si>
+  <si>
+    <t>Density</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DE8AB8-9AAE-4599-9FDD-F3E7F32F9B0A}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E1" sqref="E1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.625" defaultRowHeight="14.25"/>
@@ -435,7 +438,7 @@
     <col min="3" max="4" width="3.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -448,8 +451,11 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -462,8 +468,11 @@
       <c r="D2">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>0.28356481</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -476,8 +485,11 @@
       <c r="D3">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>0.28356481</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -490,8 +502,11 @@
       <c r="D4">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>0.28356481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -504,8 +519,11 @@
       <c r="D5">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>0.28356481</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -518,8 +536,11 @@
       <c r="D6">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>0.28356481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -532,8 +553,11 @@
       <c r="D7">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>0.28356481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -545,6 +569,9 @@
       </c>
       <c r="D8">
         <v>110</v>
+      </c>
+      <c r="E8">
+        <v>0.28356481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>